<commit_message>
Update on 20250525 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -512,10 +512,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>卫视,深圳市,汕头市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>新疆</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -614,6 +610,10 @@
   </si>
   <si>
     <t>yy.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,深圳市,部分广东频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -711,16 +711,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1045,7 +1066,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1054,22 +1075,22 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1083,7 +1104,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1095,7 +1116,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1156,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1149,7 +1170,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1161,7 +1182,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1175,7 +1196,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1183,11 +1204,11 @@
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1199,7 +1220,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1239,7 +1260,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1253,7 +1274,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1265,7 +1286,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1279,29 +1300,29 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1313,7 +1334,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="1" t="s">
         <v>64</v>
       </c>
@@ -1325,29 +1346,29 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1356,22 +1377,22 @@
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
@@ -1398,20 +1419,20 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>147</v>
-      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1425,7 +1446,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="6"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1437,7 +1458,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1477,69 +1498,69 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="7"/>
+      <c r="B37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="6"/>
-      <c r="B37" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="7"/>
+      <c r="B38" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="6"/>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="7"/>
+      <c r="B39" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1553,17 +1574,17 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="6"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="6"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="1" t="s">
         <v>95</v>
       </c>
@@ -1575,7 +1596,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="6"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="1" t="s">
         <v>96</v>
       </c>
@@ -1587,27 +1608,27 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="6"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="1" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="7"/>
+      <c r="B46" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="6"/>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
@@ -1626,21 +1647,21 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="6" t="s">
-        <v>126</v>
+      <c r="A49" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>104</v>
@@ -1648,22 +1669,22 @@
       <c r="C49" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="6"/>
+      <c r="A50" s="7"/>
       <c r="B50" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="7"/>
+      <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1672,32 +1693,32 @@
       <c r="C51" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="6"/>
+      <c r="A52" s="7"/>
       <c r="B52" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="7"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="6"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="7"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -1711,29 +1732,29 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="6"/>
+      <c r="A55" s="7"/>
       <c r="B55" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="6" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="6"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D56" s="7"/>
+      <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="6"/>
+      <c r="A57" s="7"/>
       <c r="B57" s="1" t="s">
         <v>116</v>
       </c>
@@ -1745,7 +1766,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="6"/>
+      <c r="A58" s="7"/>
       <c r="B58" s="1" t="s">
         <v>120</v>
       </c>
@@ -1759,6 +1780,18 @@
   </sheetData>
   <autoFilter ref="A1:D57"/>
   <mergeCells count="21">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D24:D25"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A41:A46"/>
@@ -1768,21 +1801,10 @@
     <mergeCell ref="D51:D53"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1844,16 +1866,16 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250526 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="154">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -520,10 +520,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xizang.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>西藏自治区频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -614,6 +610,18 @@
   </si>
   <si>
     <t>卫视,深圳市,部分广东频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tibet.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanxifenyang.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汾阳市频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -662,7 +670,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -685,13 +693,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -711,37 +756,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1038,14 +1071,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
@@ -1066,7 +1099,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1075,22 +1108,22 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="7"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1104,7 +1137,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1149,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1156,7 +1189,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1170,7 +1203,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1182,7 +1215,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1196,7 +1229,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1204,11 +1237,11 @@
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1220,7 +1253,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1260,7 +1293,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1274,7 +1307,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1286,7 +1319,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1300,29 +1333,29 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
       <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1334,7 +1367,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="7"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="1" t="s">
         <v>64</v>
       </c>
@@ -1346,29 +1379,29 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="7" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1377,22 +1410,22 @@
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="7"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
@@ -1419,20 +1452,20 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1446,7 +1479,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1458,7 +1491,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1498,69 +1531,69 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="6"/>
+      <c r="B37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="7"/>
-      <c r="B37" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="6"/>
+      <c r="B38" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="7"/>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="6"/>
+      <c r="B39" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="7"/>
-      <c r="B39" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="8" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1574,17 +1607,17 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="7"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="7"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="1" t="s">
         <v>95</v>
       </c>
@@ -1596,7 +1629,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="7"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="1" t="s">
         <v>96</v>
       </c>
@@ -1608,199 +1641,211 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="7"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D45" s="1" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="9"/>
+      <c r="B46" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="7"/>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="A47" s="10"/>
       <c r="B47" s="1" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="7" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D50" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="7"/>
-      <c r="B50" s="1" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="6"/>
+      <c r="B51" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="6"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="7" t="s">
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D52" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="7"/>
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="6"/>
+      <c r="B53" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="6"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="7"/>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="6"/>
+      <c r="B54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="7" t="s">
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="7"/>
-      <c r="B55" s="1" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="6"/>
+      <c r="B56" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D56" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="7"/>
-      <c r="B56" s="1" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="6"/>
+      <c r="B57" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="7"/>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" s="6"/>
+      <c r="B58" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="7"/>
-      <c r="B58" s="1" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" s="6"/>
+      <c r="B59" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="1" t="s">
+      <c r="C59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D57"/>
+  <autoFilter ref="A1:D59"/>
   <mergeCells count="21">
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D24:D25"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="A54:A58"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1866,16 +1911,16 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250526 part 6
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="156">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -439,84 +439,190 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>yunnan.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qicaiyunnan.js</t>
+  </si>
+  <si>
+    <t>yn.js</t>
+  </si>
+  <si>
+    <t>卫视,云南省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhejiang.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,浙江省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hangzhou.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杭州市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hztv.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ningbo.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宁波市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合肥市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浙江嵊泗,普陀频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhejiangdf.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>辽宁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shenzhen.js</t>
+  </si>
+  <si>
+    <t>shenzhen.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大连市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shaanxi2.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地,网络(feylen提供)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地</t>
+  </si>
+  <si>
+    <t>xian.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tongchuan.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西安市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铜川市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>山东</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinan.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>济南市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanxi.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanxidf.js</t>
+  </si>
+  <si>
+    <t>山西地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baode.js</t>
+  </si>
+  <si>
+    <t>保德频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>江苏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jstv.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,江苏省频道和江苏地方频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YY的直播间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地,网络(feylen提供)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yy.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,深圳市,部分广东频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tibet.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanxifenyang.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汾阳市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wlmq.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乌鲁木齐市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>卫视,新疆维吾尔自治区频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>yunnan.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>qicaiyunnan.js</t>
-  </si>
-  <si>
-    <t>yn.js</t>
-  </si>
-  <si>
-    <t>卫视,云南省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhejiang.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,浙江省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hangzhou.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>杭州市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hztv.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ningbo.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宁波市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合肥市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>浙江嵊泗,普陀频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zhejiangdf.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>辽宁</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shenzhen.js</t>
-  </si>
-  <si>
-    <t>shenzhen.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大连市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>新疆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>西藏</t>
+    <t>新疆
+维吾尔自治区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -524,104 +630,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>shaanxi2.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本地,网络(feylen提供)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本地</t>
-  </si>
-  <si>
-    <t>xian.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tongchuan.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>西安市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>铜川市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>山东</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jinan.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>济南市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shanxi.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shanxidf.js</t>
-  </si>
-  <si>
-    <t>山西地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>baode.js</t>
-  </si>
-  <si>
-    <t>保德频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>江苏</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jstv.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,江苏省频道和江苏地方频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YY的直播间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本地,网络(feylen提供)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>yy.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,深圳市,部分广东频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tibet.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shanxifenyang.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>汾阳市频道</t>
+    <t>西藏
+自治区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -736,7 +746,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -756,10 +766,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -769,6 +782,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,7 +1096,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1099,7 +1124,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1113,7 +1138,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1123,7 +1148,7 @@
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1137,7 +1162,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1145,11 +1170,11 @@
         <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1189,7 +1214,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1203,7 +1228,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1215,21 +1240,21 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1237,11 +1262,11 @@
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1253,7 +1278,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="6"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1293,7 +1318,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1307,7 +1332,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="6"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1319,7 +1344,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1333,7 +1358,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
@@ -1345,7 +1370,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
@@ -1355,7 +1380,7 @@
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="6"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1367,7 +1392,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="6"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="1" t="s">
         <v>64</v>
       </c>
@@ -1379,7 +1404,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="6"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
@@ -1391,7 +1416,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="6"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
@@ -1401,7 +1426,7 @@
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1415,7 +1440,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="6"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
@@ -1425,7 +1450,7 @@
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="6"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
@@ -1452,20 +1477,20 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1479,7 +1504,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="6"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1491,7 +1516,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="6"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1504,16 +1529,16 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
@@ -1531,73 +1556,73 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="6"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="8"/>
+      <c r="B38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="8"/>
+      <c r="B39" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="6"/>
-      <c r="B38" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="9" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>23</v>
@@ -1607,17 +1632,17 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="1" t="s">
         <v>95</v>
       </c>
@@ -1629,7 +1654,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="1" t="s">
         <v>96</v>
       </c>
@@ -1641,39 +1666,39 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="10"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
@@ -1690,23 +1715,23 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="4" t="s">
-        <v>126</v>
+    <row r="49" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A49" s="12" t="s">
+        <v>155</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="6" t="s">
-        <v>125</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>104</v>
@@ -1715,11 +1740,11 @@
         <v>42</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="6"/>
+      <c r="A51" s="14"/>
       <c r="B51" s="1" t="s">
         <v>105</v>
       </c>
@@ -1729,123 +1754,135 @@
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="15"/>
+      <c r="B52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="8"/>
+      <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D52" s="7" t="s">
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="8"/>
+      <c r="B55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="6"/>
-      <c r="B53" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="6"/>
-      <c r="B54" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="7"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" s="1" t="s">
+      <c r="C56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="1" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="8"/>
+      <c r="B57" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="6"/>
-      <c r="B56" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="1" t="s">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" s="8"/>
+      <c r="B58" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" s="8"/>
+      <c r="B59" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="6"/>
-      <c r="B57" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="7"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="6"/>
-      <c r="B58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="6"/>
-      <c r="B59" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="1" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A60" s="8"/>
+      <c r="B60" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D59"/>
+  <autoFilter ref="A1:D60"/>
   <mergeCells count="21">
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A11:A14"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A50:A52"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1911,16 +1948,16 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update on 20250528 part 3
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="158">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -632,6 +632,14 @@
   <si>
     <t>西藏
 自治区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sichuan1.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视,四川省频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -769,10 +777,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,9 +793,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1096,7 +1104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1133,7 +1141,7 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1145,7 +1153,7 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
@@ -1365,7 +1373,7 @@
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1377,7 +1385,7 @@
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="8"/>
@@ -1411,7 +1419,7 @@
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="9" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1423,7 +1431,7 @@
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
@@ -1435,7 +1443,7 @@
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1447,7 +1455,7 @@
       <c r="C27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="8"/>
@@ -1565,7 +1573,7 @@
       <c r="C36" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="9" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1577,7 +1585,7 @@
       <c r="C37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="8"/>
@@ -1618,7 +1626,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1632,7 +1640,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="10"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="1" t="s">
         <v>134</v>
       </c>
@@ -1642,7 +1650,7 @@
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="10"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="1" t="s">
         <v>95</v>
       </c>
@@ -1654,7 +1662,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="10"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="1" t="s">
         <v>96</v>
       </c>
@@ -1666,7 +1674,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="10"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="1" t="s">
         <v>135</v>
       </c>
@@ -1678,7 +1686,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="10"/>
+      <c r="A46" s="11"/>
       <c r="B46" s="1" t="s">
         <v>137</v>
       </c>
@@ -1690,7 +1698,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="11"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="1" t="s">
         <v>148</v>
       </c>
@@ -1702,187 +1710,200 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="10" t="s">
         <v>99</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="12"/>
+      <c r="B49" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A49" s="12" t="s">
+    <row r="50" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A50" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="13" t="s">
+    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="14"/>
-      <c r="B51" s="1" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="14"/>
+      <c r="B52" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="15"/>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="9"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="15"/>
+      <c r="B53" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="6" t="s">
+      <c r="C53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="8" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D54" s="9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="8"/>
-      <c r="B54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="8"/>
       <c r="B55" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="8"/>
+      <c r="B56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="8" t="s">
+      <c r="C56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="9"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="C57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="8"/>
-      <c r="B57" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="8"/>
       <c r="B58" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="8"/>
       <c r="B59" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="8"/>
       <c r="B60" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="8"/>
+      <c r="B61" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="C61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D60"/>
-  <mergeCells count="21">
+  <autoFilter ref="A1:D61"/>
+  <mergeCells count="22">
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D24:D25"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="A50:A52"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250530 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$62</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="159">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -640,6 +640,10 @@
   </si>
   <si>
     <t>卫视,四川省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shanxi_new.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -754,7 +758,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -780,10 +784,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -802,6 +806,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,7 +1117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1132,7 +1145,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1141,22 +1154,22 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1170,7 +1183,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1182,7 +1195,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1222,7 +1235,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1236,7 +1249,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1248,7 +1261,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1262,7 +1275,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1274,7 +1287,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>44</v>
       </c>
@@ -1286,7 +1299,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
@@ -1326,7 +1339,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1340,7 +1353,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1352,7 +1365,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1366,29 +1379,29 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="8"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1400,7 +1413,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="1" t="s">
         <v>64</v>
       </c>
@@ -1412,29 +1425,29 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1443,22 +1456,22 @@
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
@@ -1498,7 +1511,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1512,7 +1525,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1524,7 +1537,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1564,7 +1577,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1573,22 +1586,22 @@
       <c r="C36" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="8"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="9"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="8"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="1" t="s">
         <v>127</v>
       </c>
@@ -1600,7 +1613,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="8"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="1" t="s">
         <v>128</v>
       </c>
@@ -1635,7 +1648,7 @@
       <c r="C41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="16" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1647,263 +1660,274 @@
       <c r="C42" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="11"/>
       <c r="B43" s="1" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D43" s="18"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="11"/>
       <c r="B44" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="11"/>
       <c r="B45" s="1" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="11"/>
       <c r="B46" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="12"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="10" t="s">
-        <v>99</v>
-      </c>
+      <c r="A48" s="12"/>
       <c r="B48" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="12"/>
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="12"/>
+      <c r="B50" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
+      <c r="A51" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="13" t="s">
+    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D52" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="14"/>
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="14"/>
+      <c r="B53" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="9"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="15"/>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="15"/>
+      <c r="B54" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="6" t="s">
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="8" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D55" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="8"/>
-      <c r="B55" s="1" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="9"/>
+      <c r="B56" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="8"/>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="9"/>
+      <c r="B57" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="8" t="s">
+      <c r="C57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="8"/>
-      <c r="B58" s="1" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" s="9"/>
+      <c r="B59" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D59" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="8"/>
-      <c r="B59" s="1" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A60" s="9"/>
+      <c r="B60" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="9"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="8"/>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="9"/>
+      <c r="B61" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="8"/>
-      <c r="B61" s="1" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" s="9"/>
+      <c r="B62" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D61"/>
-  <mergeCells count="22">
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A48:A49"/>
+  <autoFilter ref="A1:D62"/>
+  <mergeCells count="23">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A11:A14"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A26:A28"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="A58:A62"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="D41:D43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250611 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="166">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -621,20 +621,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>新疆
-维吾尔自治区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>西藏自治区频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>西藏
-自治区</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sichuan1.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -652,6 +642,34 @@
   </si>
   <si>
     <t>卫视,山东省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quanzhou.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泉州市频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>香港</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKS.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卫视</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西藏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新疆</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -700,7 +718,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -723,50 +741,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -786,9 +767,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -797,32 +775,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1125,7 +1085,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1139,7 +1099,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1153,7 +1113,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1167,7 +1127,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1177,7 +1137,7 @@
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1191,7 +1151,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1203,7 +1163,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1215,7 +1175,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1229,7 +1189,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1243,712 +1203,739 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="8"/>
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="10"/>
+      <c r="B11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="8"/>
+      <c r="A12" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="10"/>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="8"/>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="10"/>
+      <c r="B14" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="8"/>
-      <c r="B14" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="4" t="s">
-        <v>50</v>
+      <c r="A16" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="8"/>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="10"/>
+      <c r="B19" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="8"/>
+      <c r="A20" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="10"/>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="8"/>
-      <c r="B21" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="10"/>
+      <c r="B22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="8"/>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="10"/>
+      <c r="B23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="8"/>
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="10"/>
+      <c r="B24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="8"/>
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="10"/>
+      <c r="B25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="8"/>
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="10"/>
+      <c r="B26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="8"/>
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="10"/>
+      <c r="B28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="8"/>
-      <c r="B28" s="1" t="s">
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="10"/>
+      <c r="B29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="8" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="8"/>
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="10"/>
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="8"/>
-      <c r="B33" s="1" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="10"/>
+      <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="8" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="8"/>
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="10"/>
+      <c r="B38" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="8"/>
-      <c r="B38" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="8"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="10" t="s">
-        <v>131</v>
-      </c>
+      <c r="A40" s="10"/>
       <c r="B40" s="1" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="12"/>
+      <c r="A41" s="10" t="s">
+        <v>131</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="10"/>
+      <c r="B42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="10" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D43" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="11"/>
-      <c r="B43" s="1" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="10"/>
+      <c r="B44" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="11"/>
-      <c r="B44" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="18"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="11"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="10"/>
+      <c r="B46" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="11"/>
-      <c r="B46" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="10"/>
+      <c r="B47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="11"/>
-      <c r="B47" s="1" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="10"/>
+      <c r="B48" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="11"/>
-      <c r="B48" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="12"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="10" t="s">
-        <v>99</v>
-      </c>
+      <c r="A50" s="10"/>
       <c r="B50" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="12"/>
+      <c r="A51" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="B51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="10"/>
+      <c r="B52" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="37.5" x14ac:dyDescent="0.15">
-      <c r="A52" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="13" t="s">
+      <c r="C53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D54" s="9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="14"/>
-      <c r="B54" s="1" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="11"/>
+      <c r="B55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="15"/>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="11"/>
+      <c r="B56" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="6" t="s">
+      <c r="C56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="8" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D57" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="8"/>
-      <c r="B57" s="1" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" s="10"/>
+      <c r="B58" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="9"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="8"/>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" s="10"/>
+      <c r="B59" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="9"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="8" t="s">
+      <c r="C59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A60" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="8"/>
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="10"/>
+      <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D61" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="8"/>
-      <c r="B61" s="1" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" s="10"/>
+      <c r="B62" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="9"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="8"/>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A63" s="10"/>
+      <c r="B63" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="8"/>
-      <c r="B63" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" s="10"/>
+      <c r="B64" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>118</v>
       </c>
     </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A65" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D63"/>
-  <mergeCells count="24">
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A9:A10"/>
+  <autoFilter ref="A1:D64"/>
+  <mergeCells count="25">
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20250616 part 5
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -12,15 +12,15 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$64</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="133">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,22 +62,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>migu.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络(feylen提供)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1905电影网</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>央视,部分卫视和部分地方台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>平台</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -114,10 +102,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本地,网络(feylen提供)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>anhuidf.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,10 +122,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>咪咕</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>福建</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -177,10 +157,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>贵州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gztv.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -189,48 +165,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>网络(feylen提供)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>广州市频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>foshan.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dongguan.js</t>
-  </si>
-  <si>
-    <t>佛山市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>东莞市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gzdj.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,贵州省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>海南</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hainan.js</t>
-  </si>
-  <si>
-    <t>卫视,海南省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hebeidf.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -309,10 +247,6 @@
     <t>hunan.js</t>
   </si>
   <si>
-    <t>hn.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>卫视,湖南省频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -325,22 +259,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>吉林</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>江西</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>changchun.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>长春市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jxtv.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -349,33 +271,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jiujiang.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jazh.js</t>
   </si>
   <si>
-    <t>九江市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>吉安市频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>青海</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>qinghai.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>卫视,青海省频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>陕西</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -396,22 +298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>yangquan.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>datong.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阳泉市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大同市频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>四川</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -431,18 +317,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xinjiang.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>xjtv.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>yunnan.js</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>qicaiyunnan.js</t>
   </si>
   <si>
@@ -512,10 +390,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本地,网络(feylen提供)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>本地</t>
   </si>
   <si>
@@ -561,10 +435,6 @@
     <t>baode.js</t>
   </si>
   <si>
-    <t>保德频道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>江苏</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -585,10 +455,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本地,网络(feylen提供)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>yy.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -670,6 +536,10 @@
   </si>
   <si>
     <t>新疆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保德县频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -718,7 +588,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -741,13 +611,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -782,6 +678,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1085,7 +1002,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1093,14 +1010,14 @@
   <cols>
     <col min="1" max="1" width="19.375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1122,8 +1039,8 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>20</v>
+      <c r="D2" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -1134,808 +1051,660 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
+      <c r="A14" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="10"/>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="10"/>
+      <c r="B18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="10" t="s">
-        <v>56</v>
-      </c>
+      <c r="A20" s="10"/>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>60</v>
+        <v>6</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="10"/>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="10"/>
+      <c r="A23" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>63</v>
+      <c r="D23" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="10"/>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="1" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="10"/>
-      <c r="B25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="10"/>
-      <c r="B26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="10"/>
-      <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="10"/>
-      <c r="B29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="A30" s="10"/>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
-        <v>139</v>
-      </c>
+      <c r="A31" s="10"/>
       <c r="B31" s="1" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="10" t="s">
-        <v>78</v>
-      </c>
+      <c r="A32" s="10"/>
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="10"/>
+      <c r="A33" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="10"/>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="7" t="s">
-        <v>120</v>
+      <c r="A35" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>123</v>
+        <v>94</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="A36" s="10"/>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>89</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="10" t="s">
-        <v>90</v>
-      </c>
+      <c r="A37" s="10"/>
       <c r="B37" s="1" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>93</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="10"/>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D38" s="9"/>
+        <v>94</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="10"/>
       <c r="B39" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="10"/>
       <c r="B40" s="1" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="10" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="10"/>
       <c r="B42" s="1" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="10" t="s">
-        <v>91</v>
+      <c r="A43" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>94</v>
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="10"/>
+      <c r="A44" s="17" t="s">
+        <v>131</v>
+      </c>
       <c r="B44" s="1" t="s">
-        <v>134</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="10"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="1" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D45" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="10"/>
+      <c r="A46" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>97</v>
+        <v>6</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="10"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="1" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>98</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D47" s="13"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="10"/>
+      <c r="A48" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="B48" s="1" t="s">
-        <v>135</v>
+        <v>79</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>136</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="10"/>
       <c r="B49" s="1" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>138</v>
+        <v>94</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="10"/>
       <c r="B50" s="1" t="s">
-        <v>148</v>
+        <v>83</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>149</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="10" t="s">
-        <v>99</v>
-      </c>
+      <c r="A51" s="10"/>
       <c r="B51" s="1" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="10"/>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="6" t="s">
-        <v>164</v>
+      <c r="A53" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A55" s="11"/>
-      <c r="B55" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="9"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A56" s="11"/>
-      <c r="B56" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="10"/>
-      <c r="B58" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="9"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="10"/>
-      <c r="B59" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="9"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="10"/>
-      <c r="B61" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A62" s="10"/>
-      <c r="B62" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="9"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A63" s="10"/>
-      <c r="B63" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A64" s="10"/>
-      <c r="B64" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D64"/>
-  <mergeCells count="25">
+  <autoFilter ref="A1:D52"/>
+  <mergeCells count="23">
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1945,7 +1714,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1953,13 +1722,13 @@
   <cols>
     <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1973,7 +1742,7 @@
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -1987,7 +1756,7 @@
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1996,39 +1765,25 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D5"/>
+  <autoFilter ref="A1:D4"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update on 20250708 part 12
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="地方台JS脚本" sheetId="1" r:id="rId1"/>
     <sheet name="其他JS脚本" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$52</definedName>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="135">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -540,6 +539,14 @@
   </si>
   <si>
     <t>保德县频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phoenix.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>凤凰中文,资讯和香港频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -588,7 +595,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -611,39 +618,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -678,28 +659,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1002,7 +965,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1039,7 +1002,7 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1051,7 +1014,7 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
@@ -1231,7 +1194,7 @@
       <c r="C17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1243,7 +1206,7 @@
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
@@ -1277,7 +1240,7 @@
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1289,7 +1252,7 @@
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
@@ -1301,7 +1264,7 @@
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1381,7 +1344,7 @@
       <c r="C29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1393,7 +1356,7 @@
       <c r="C30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
@@ -1455,7 +1418,7 @@
       <c r="C35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1467,7 +1430,7 @@
       <c r="C36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="11"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="10"/>
@@ -1477,7 +1440,7 @@
       <c r="C37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="11"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="10"/>
@@ -1556,7 +1519,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="11" t="s">
         <v>131</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1565,12 +1528,12 @@
       <c r="C44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="18"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="1" t="s">
         <v>116</v>
       </c>
@@ -1582,7 +1545,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -1591,19 +1554,19 @@
       <c r="C46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="16"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="13"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="10" t="s">
@@ -1627,7 +1590,7 @@
       <c r="C49" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="D49" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1639,7 +1602,7 @@
       <c r="C50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="11"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="10"/>
@@ -1666,7 +1629,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="10" t="s">
         <v>127</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -1679,9 +1642,34 @@
         <v>129</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="10"/>
+      <c r="B54" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D52"/>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="A29:A32"/>
     <mergeCell ref="D49:D50"/>
@@ -1693,18 +1681,6 @@
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="D46:D47"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1788,17 +1764,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20250719 part 4
</commit_message>
<xml_diff>
--- a/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
+++ b/直播源汇总文档/其他文档/酷9脚本汇总统计.xlsx
@@ -11,7 +11,7 @@
     <sheet name="其他JS脚本" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">地方台JS脚本!$A$1:$D$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">其他JS脚本!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
   <si>
     <t>JS脚本名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,10 +45,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本地</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1905.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -389,9 +385,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本地</t>
-  </si>
-  <si>
     <t>xian.js</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -548,6 +541,21 @@
   <si>
     <t>凤凰中文,资讯和香港频道</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贵州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贵州省频道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gzstv.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本地,Github远程</t>
   </si>
 </sst>
 </file>
@@ -624,7 +632,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -653,16 +661,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -965,7 +976,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -973,14 +984,14 @@
   <cols>
     <col min="1" max="1" width="19.375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -993,694 +1004,708 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="9"/>
+        <v>136</v>
+      </c>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" s="11"/>
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" s="11"/>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="10"/>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="11"/>
+      <c r="B9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" s="11"/>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" s="11"/>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" s="11"/>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="11"/>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="11"/>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="11"/>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="11"/>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="11"/>
+      <c r="B22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A23" s="11"/>
+      <c r="B23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="11"/>
+      <c r="B25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="11"/>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A31" s="11"/>
+      <c r="B31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="11"/>
+      <c r="B32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="11"/>
+      <c r="B33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="10"/>
-      <c r="B9" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="11"/>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="11"/>
+      <c r="B37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="11"/>
+      <c r="B38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="11"/>
+      <c r="B39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A40" s="11"/>
+      <c r="B40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A41" s="11"/>
+      <c r="B41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A42" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="11"/>
+      <c r="B43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="13"/>
+      <c r="B46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="11"/>
+      <c r="B48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="11"/>
+      <c r="B50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="11"/>
+      <c r="B51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" s="12"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="11"/>
+      <c r="B52" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="11"/>
+      <c r="B53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="10"/>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="10"/>
-      <c r="B13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="10"/>
-      <c r="B15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="10"/>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="10"/>
-      <c r="B19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="10"/>
-      <c r="B20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="10"/>
-      <c r="B21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="10"/>
-      <c r="B22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="10"/>
-      <c r="B24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="10"/>
-      <c r="B27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="10"/>
-      <c r="B30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="10"/>
-      <c r="B31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="10"/>
-      <c r="B32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="10"/>
-      <c r="B34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="10"/>
-      <c r="B36" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="10"/>
-      <c r="B37" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="10"/>
-      <c r="B38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="10"/>
-      <c r="B39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="11"/>
+      <c r="B55" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="10"/>
-      <c r="B40" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="10"/>
-      <c r="B42" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="11"/>
-      <c r="B45" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="10"/>
-      <c r="B47" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="10"/>
-      <c r="B49" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="10"/>
-      <c r="B50" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="9"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="10"/>
-      <c r="B51" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="10"/>
-      <c r="B52" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="10"/>
-      <c r="B54" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D52"/>
+  <autoFilter ref="A1:D53"/>
   <mergeCells count="24">
-    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A54:A55"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="D50:D51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1698,13 +1723,13 @@
   <cols>
     <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1718,44 +1743,44 @@
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>